<commit_message>
add ec2 info and increase reactive logic
</commit_message>
<xml_diff>
--- a/data-set/i-00d430fd136bd05c9.xlsx
+++ b/data-set/i-00d430fd136bd05c9.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,6 +492,846 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>14:31:11</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>4987.0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>4213.0</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>14:32:21</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>3430.0</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>3100.0</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>14:32:51</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>3430.0</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>3100.0</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>14:33:15</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>2.2951</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>3224.0</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2836.0</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>14:33:39</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>2.2951</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>3224.0</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2836.0</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>14:33:57</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>2.2951</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>3224.0</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2836.0</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>14:34:04</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>4507.0</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>11277.0</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>14:34:28</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>4507.0</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>11277.0</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>14:34:51</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>4507.0</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>11277.0</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>14:35:15</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>3420.0</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>5692.0</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>14:35:39</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>3520.0</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>3284.0</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>14:36:03</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>3520.0</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>3284.0</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>14:36:27</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>3430.0</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>14:36:50</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>3430.0</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>14:37:14</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>3430.0</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>14:37:38</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>3430.0</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>14:38:02</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>3364.0</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>3100.0</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>14:38:25</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>3364.0</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>3100.0</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>14:38:49</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>3364.0</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>3100.0</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>14:39:13</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>3576.0</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>3204.0</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>14:39:37</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>2.1311</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>3576.0</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>3204.0</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>14:40:01</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>2.1311</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>3644.0</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>3140.0</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>14:40:20</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>2.1311</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>3644.0</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>3140.0</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>14:40:46</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>2.1311</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>6122.0</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>6017.0</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>14:41:12</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>2.3729</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>6122.0</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>6017.0</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>14:41:41</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>2.3729</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>6122.0</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>6017.0</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>14:42:07</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>2.2034</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>3498.0</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>3036.0</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>14:42:34</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>2.2034</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>3498.0</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>3036.0</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>